<commit_message>
move negative to actual costs instead of rates
</commit_message>
<xml_diff>
--- a/TOU_analysis.xlsx
+++ b/TOU_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/389d50da7730b885/Documents/TOU_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{F0E87120-3E09-C340-AB62-B85760477DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{849CAE3B-02D6-0142-8AC0-15FE20AEC3E3}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{F0E87120-3E09-C340-AB62-B85760477DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34AB12F5-9F28-1A48-9CB8-D831EA17DABA}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="2540" windowWidth="32160" windowHeight="23820" xr2:uid="{1A87D379-06A0-BC40-A650-8DF4C831EFEF}"/>
   </bookViews>
@@ -225,7 +225,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,6 +360,12 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -637,7 +643,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -714,24 +720,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="9" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="21" fillId="16" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="21" fillId="16" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="22" fillId="16" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="22" fillId="16" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
@@ -1092,7 +1099,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1595,52 +1602,52 @@
         <v>28</v>
       </c>
       <c r="D21" s="25">
-        <f>SUMPRODUCT(D$7:D$8,D$15:D$16)/SUM(D$15:D$16)*-1</f>
-        <v>-9.6767500000000006E-2</v>
+        <f>SUMPRODUCT(D$7:D$8,D$15:D$16)/SUM(D$15:D$16)</f>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="E21" s="25">
-        <f t="shared" ref="E21:O21" si="1">SUMPRODUCT(E$7:E$8,E$15:E$16)/SUM(E$15:E$16)*-1</f>
-        <v>-9.6767500000000006E-2</v>
+        <f t="shared" ref="E21:O21" si="1">SUMPRODUCT(E$7:E$8,E$15:E$16)/SUM(E$15:E$16)</f>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="F21" s="25">
         <f t="shared" si="1"/>
-        <v>-9.6767500000000006E-2</v>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="G21" s="25">
         <f t="shared" si="1"/>
-        <v>-9.6767500000000006E-2</v>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="H21" s="25">
         <f t="shared" si="1"/>
-        <v>-9.6767500000000006E-2</v>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="I21" s="25">
         <f t="shared" si="1"/>
-        <v>-0.11232249999999999</v>
+        <v>0.11232249999999999</v>
       </c>
       <c r="J21" s="25">
         <f t="shared" si="1"/>
-        <v>-0.11232249999999999</v>
+        <v>0.11232249999999999</v>
       </c>
       <c r="K21" s="25">
         <f t="shared" si="1"/>
-        <v>-0.11232249999999999</v>
+        <v>0.11232249999999999</v>
       </c>
       <c r="L21" s="25">
         <f t="shared" si="1"/>
-        <v>-0.11232249999999999</v>
+        <v>0.11232249999999999</v>
       </c>
       <c r="M21" s="25">
         <f t="shared" si="1"/>
-        <v>-9.6767500000000006E-2</v>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="N21" s="25">
         <f t="shared" si="1"/>
-        <v>-9.6767500000000006E-2</v>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="O21" s="25">
         <f t="shared" si="1"/>
-        <v>-9.6767500000000006E-2</v>
+        <v>9.6767500000000006E-2</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>15</v>
@@ -1654,52 +1661,52 @@
         <v>28</v>
       </c>
       <c r="D22" s="25">
-        <f>D9*-1</f>
-        <v>-8.5699999999999998E-2</v>
+        <f>D9</f>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="E22" s="25">
-        <f t="shared" ref="E22:O22" si="2">E9*-1</f>
-        <v>-8.5699999999999998E-2</v>
+        <f t="shared" ref="E22:O22" si="2">E9</f>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="F22" s="25">
         <f t="shared" si="2"/>
-        <v>-8.5699999999999998E-2</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="G22" s="25">
         <f t="shared" si="2"/>
-        <v>-8.5699999999999998E-2</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="H22" s="25">
         <f t="shared" si="2"/>
-        <v>-8.5699999999999998E-2</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="I22" s="25">
         <f t="shared" si="2"/>
-        <v>-0.1038</v>
+        <v>0.1038</v>
       </c>
       <c r="J22" s="25">
         <f t="shared" si="2"/>
-        <v>-0.1038</v>
+        <v>0.1038</v>
       </c>
       <c r="K22" s="25">
         <f t="shared" si="2"/>
-        <v>-0.1038</v>
+        <v>0.1038</v>
       </c>
       <c r="L22" s="25">
         <f t="shared" si="2"/>
-        <v>-0.1038</v>
+        <v>0.1038</v>
       </c>
       <c r="M22" s="25">
         <f t="shared" si="2"/>
-        <v>-8.5699999999999998E-2</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="N22" s="25">
         <f t="shared" si="2"/>
-        <v>-8.5699999999999998E-2</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="O22" s="25">
         <f t="shared" si="2"/>
-        <v>-8.5699999999999998E-2</v>
+        <v>8.5699999999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
@@ -1710,11 +1717,11 @@
         <v>36</v>
       </c>
       <c r="D24" s="26">
-        <f t="shared" ref="D24:O24" si="3">D$21*D$17</f>
+        <f>(D$21*D$17)*-1</f>
         <v>-83.220050000000001</v>
       </c>
       <c r="E24" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E24:O24" si="3">(E$21*E$17)*-1</f>
         <v>-119.5078625</v>
       </c>
       <c r="F24" s="26">
@@ -1773,11 +1780,11 @@
         <v>36</v>
       </c>
       <c r="D25" s="26">
-        <f t="shared" ref="D25:O25" si="4">D$22*D$17</f>
+        <f>D$22*D$17*-1</f>
         <v>-73.701999999999998</v>
       </c>
       <c r="E25" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E25:O25" si="4">E$22*E$17*-1</f>
         <v>-105.8395</v>
       </c>
       <c r="F25" s="26">
@@ -1829,61 +1836,61 @@
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="47" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="57">
+      <c r="D26" s="58">
         <f t="shared" ref="D26:O26" si="5">D24-D25</f>
         <v>-9.5180500000000023</v>
       </c>
-      <c r="E26" s="57">
+      <c r="E26" s="58">
         <f t="shared" si="5"/>
         <v>-13.668362500000001</v>
       </c>
-      <c r="F26" s="57">
+      <c r="F26" s="58">
         <f t="shared" si="5"/>
         <v>-16.291360000000026</v>
       </c>
-      <c r="G26" s="57">
+      <c r="G26" s="58">
         <f t="shared" si="5"/>
         <v>-11.676212500000005</v>
       </c>
-      <c r="H26" s="57">
+      <c r="H26" s="58">
         <f t="shared" si="5"/>
         <v>-7.8689925000000045</v>
       </c>
-      <c r="I26" s="57">
+      <c r="I26" s="58">
         <f t="shared" si="5"/>
         <v>-4.2953399999999888</v>
       </c>
-      <c r="J26" s="57">
+      <c r="J26" s="58">
         <f t="shared" si="5"/>
         <v>-8.3009149999999892</v>
       </c>
-      <c r="K26" s="57">
+      <c r="K26" s="58">
         <f t="shared" si="5"/>
         <v>-5.624849999999995</v>
       </c>
-      <c r="L26" s="57">
+      <c r="L26" s="58">
         <f t="shared" si="5"/>
         <v>-6.860612500000002</v>
       </c>
-      <c r="M26" s="57">
+      <c r="M26" s="58">
         <f t="shared" si="5"/>
         <v>-8.9646749999999997</v>
       </c>
-      <c r="N26" s="57">
+      <c r="N26" s="58">
         <f t="shared" si="5"/>
         <v>-6.2531375000000082</v>
       </c>
-      <c r="O26" s="57">
+      <c r="O26" s="58">
         <f t="shared" si="5"/>
         <v>-8.278490000000005</v>
       </c>
-      <c r="P26" s="58">
+      <c r="P26" s="59">
         <f>SUM(D26:O26)</f>
         <v>-107.60099750000002</v>
       </c>
@@ -1910,22 +1917,22 @@
       <c r="P27" s="41"/>
     </row>
     <row r="28" spans="2:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
     </row>
     <row r="29" spans="2:18" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
@@ -2307,55 +2314,55 @@
       <c r="C42" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="49">
+      <c r="D42" s="50">
         <f t="shared" ref="D42:O42" si="19">D$39*D$35</f>
         <v>0</v>
       </c>
-      <c r="E42" s="49">
+      <c r="E42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F42" s="49">
+      <c r="F42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="G42" s="49">
+      <c r="G42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="H42" s="49">
+      <c r="H42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="I42" s="49">
+      <c r="I42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J42" s="49">
+      <c r="J42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="K42" s="49">
+      <c r="K42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="L42" s="49">
+      <c r="L42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="M42" s="49">
+      <c r="M42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="N42" s="49">
+      <c r="N42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O42" s="49">
+      <c r="O42" s="50">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P42" s="50">
+      <c r="P42" s="51">
         <f>SUM(D42:O42)</f>
         <v>0</v>
       </c>
@@ -2364,7 +2371,7 @@
       </c>
     </row>
     <row r="43" spans="2:18" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="47" t="str">
+      <c r="B43" s="48" t="str">
         <f>_xlfn.CONCAT("Ref: ",B24)</f>
         <v>Ref: TOU Cost (Rate x Usage)</v>
       </c>
@@ -2372,62 +2379,62 @@
         <f>C24</f>
         <v>$</v>
       </c>
-      <c r="D43" s="48">
+      <c r="D43" s="49">
         <f>D24</f>
         <v>-83.220050000000001</v>
       </c>
-      <c r="E43" s="48">
+      <c r="E43" s="49">
         <f>E24</f>
         <v>-119.5078625</v>
       </c>
-      <c r="F43" s="48">
+      <c r="F43" s="49">
         <f>F24</f>
         <v>-142.44176000000002</v>
       </c>
-      <c r="G43" s="48">
+      <c r="G43" s="49">
         <f>G24</f>
         <v>-102.0897125</v>
       </c>
-      <c r="H43" s="48">
+      <c r="H43" s="49">
         <f>H24</f>
         <v>-68.801692500000001</v>
       </c>
-      <c r="I43" s="48">
+      <c r="I43" s="49">
         <f>I24</f>
         <v>-56.610539999999993</v>
       </c>
-      <c r="J43" s="48">
+      <c r="J43" s="49">
         <f>J24</f>
         <v>-109.40211499999999</v>
       </c>
-      <c r="K43" s="48">
+      <c r="K43" s="49">
         <f>K24</f>
         <v>-74.132849999999991</v>
       </c>
-      <c r="L43" s="48">
+      <c r="L43" s="49">
         <f>L24</f>
         <v>-90.419612499999999</v>
       </c>
-      <c r="M43" s="48">
+      <c r="M43" s="49">
         <f>M24</f>
         <v>-78.381675000000001</v>
       </c>
-      <c r="N43" s="48">
+      <c r="N43" s="49">
         <f>N24</f>
         <v>-54.673637500000005</v>
       </c>
-      <c r="O43" s="48">
+      <c r="O43" s="49">
         <f>O24</f>
         <v>-72.382090000000005</v>
       </c>
-      <c r="P43" s="48">
+      <c r="P43" s="49">
         <f>SUM(D43:O43)</f>
         <v>-1052.0635975</v>
       </c>
       <c r="R43" s="45"/>
     </row>
     <row r="44" spans="2:18" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="48" t="s">
         <v>55</v>
       </c>
       <c r="C44" s="14"/>
@@ -2492,55 +2499,55 @@
       <c r="C45" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="51">
+      <c r="D45" s="52">
         <f>D$40*D$35</f>
         <v>0</v>
       </c>
-      <c r="E45" s="51">
+      <c r="E45" s="52">
         <f t="shared" ref="E45:O45" si="21">E$40*E$35</f>
         <v>0</v>
       </c>
-      <c r="F45" s="51">
+      <c r="F45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="G45" s="51">
+      <c r="G45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="H45" s="51">
+      <c r="H45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="I45" s="51">
+      <c r="I45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="J45" s="51">
+      <c r="J45" s="52">
         <f>J$40*J$35</f>
         <v>0</v>
       </c>
-      <c r="K45" s="51">
+      <c r="K45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="L45" s="51">
+      <c r="L45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="M45" s="51">
+      <c r="M45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="N45" s="51">
+      <c r="N45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="O45" s="51">
+      <c r="O45" s="52">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="P45" s="51">
+      <c r="P45" s="52">
         <f>SUM(D45:O45)</f>
         <v>0</v>
       </c>
@@ -2549,7 +2556,7 @@
       </c>
     </row>
     <row r="46" spans="2:18" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="47" t="str">
+      <c r="B46" s="48" t="str">
         <f>_xlfn.CONCAT("Ref: ",B25)</f>
         <v>Ref: Flat Rate Cost (Rate X Usage)</v>
       </c>
@@ -2557,110 +2564,110 @@
         <f>C25</f>
         <v>$</v>
       </c>
-      <c r="D46" s="48">
+      <c r="D46" s="49">
         <f>D25</f>
         <v>-73.701999999999998</v>
       </c>
-      <c r="E46" s="48">
+      <c r="E46" s="49">
         <f>E25</f>
         <v>-105.8395</v>
       </c>
-      <c r="F46" s="48">
+      <c r="F46" s="49">
         <f>F25</f>
         <v>-126.15039999999999</v>
       </c>
-      <c r="G46" s="48">
+      <c r="G46" s="49">
         <f>G25</f>
         <v>-90.413499999999999</v>
       </c>
-      <c r="H46" s="48">
+      <c r="H46" s="49">
         <f>H25</f>
         <v>-60.932699999999997</v>
       </c>
-      <c r="I46" s="48">
+      <c r="I46" s="49">
         <f>I25</f>
         <v>-52.315200000000004</v>
       </c>
-      <c r="J46" s="48">
+      <c r="J46" s="49">
         <f>J25</f>
         <v>-101.10120000000001</v>
       </c>
-      <c r="K46" s="48">
+      <c r="K46" s="49">
         <f>K25</f>
         <v>-68.507999999999996</v>
       </c>
-      <c r="L46" s="48">
+      <c r="L46" s="49">
         <f>L25</f>
         <v>-83.558999999999997</v>
       </c>
-      <c r="M46" s="48">
+      <c r="M46" s="49">
         <f>M25</f>
         <v>-69.417000000000002</v>
       </c>
-      <c r="N46" s="48">
+      <c r="N46" s="49">
         <f>N25</f>
         <v>-48.420499999999997</v>
       </c>
-      <c r="O46" s="48">
+      <c r="O46" s="49">
         <f>O25</f>
         <v>-64.1036</v>
       </c>
-      <c r="P46" s="48">
+      <c r="P46" s="49">
         <f>SUM(D46:O46)</f>
         <v>-944.46260000000007</v>
       </c>
       <c r="R46" s="45"/>
     </row>
     <row r="47" spans="2:18" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="47" t="s">
+      <c r="B47" s="48" t="s">
         <v>56</v>
       </c>
       <c r="C47" s="14"/>
-      <c r="D47" s="52">
+      <c r="D47" s="53">
         <f>SUM(D45:D46)</f>
         <v>-73.701999999999998</v>
       </c>
-      <c r="E47" s="52">
+      <c r="E47" s="53">
         <f t="shared" ref="E47:O47" si="22">SUM(E45:E46)</f>
         <v>-105.8395</v>
       </c>
-      <c r="F47" s="52">
+      <c r="F47" s="53">
         <f t="shared" si="22"/>
         <v>-126.15039999999999</v>
       </c>
-      <c r="G47" s="52">
+      <c r="G47" s="53">
         <f t="shared" si="22"/>
         <v>-90.413499999999999</v>
       </c>
-      <c r="H47" s="52">
+      <c r="H47" s="53">
         <f t="shared" si="22"/>
         <v>-60.932699999999997</v>
       </c>
-      <c r="I47" s="52">
+      <c r="I47" s="53">
         <f t="shared" si="22"/>
         <v>-52.315200000000004</v>
       </c>
-      <c r="J47" s="52">
+      <c r="J47" s="53">
         <f t="shared" si="22"/>
         <v>-101.10120000000001</v>
       </c>
-      <c r="K47" s="52">
+      <c r="K47" s="53">
         <f t="shared" si="22"/>
         <v>-68.507999999999996</v>
       </c>
-      <c r="L47" s="52">
+      <c r="L47" s="53">
         <f t="shared" si="22"/>
         <v>-83.558999999999997</v>
       </c>
-      <c r="M47" s="52">
+      <c r="M47" s="53">
         <f t="shared" si="22"/>
         <v>-69.417000000000002</v>
       </c>
-      <c r="N47" s="52">
+      <c r="N47" s="53">
         <f t="shared" si="22"/>
         <v>-48.420499999999997</v>
       </c>
-      <c r="O47" s="52">
+      <c r="O47" s="53">
         <f t="shared" si="22"/>
         <v>-64.1036</v>
       </c>
@@ -2670,61 +2677,61 @@
       </c>
     </row>
     <row r="48" spans="2:18" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="47" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="57">
+      <c r="D48" s="58">
         <f>D44-D47</f>
         <v>-9.5180500000000023</v>
       </c>
-      <c r="E48" s="57">
+      <c r="E48" s="58">
         <f>E44-E47</f>
         <v>-13.668362500000001</v>
       </c>
-      <c r="F48" s="57">
+      <c r="F48" s="58">
         <f>F44-F47</f>
         <v>-16.291360000000026</v>
       </c>
-      <c r="G48" s="57">
+      <c r="G48" s="58">
         <f>G44-G47</f>
         <v>-11.676212500000005</v>
       </c>
-      <c r="H48" s="57">
+      <c r="H48" s="58">
         <f>H44-H47</f>
         <v>-7.8689925000000045</v>
       </c>
-      <c r="I48" s="57">
+      <c r="I48" s="58">
         <f>I44-I47</f>
         <v>-4.2953399999999888</v>
       </c>
-      <c r="J48" s="57">
+      <c r="J48" s="58">
         <f>J44-J47</f>
         <v>-8.3009149999999892</v>
       </c>
-      <c r="K48" s="57">
+      <c r="K48" s="58">
         <f>K44-K47</f>
         <v>-5.624849999999995</v>
       </c>
-      <c r="L48" s="57">
+      <c r="L48" s="58">
         <f>L44-L47</f>
         <v>-6.860612500000002</v>
       </c>
-      <c r="M48" s="57">
+      <c r="M48" s="58">
         <f>M44-M47</f>
         <v>-8.9646749999999997</v>
       </c>
-      <c r="N48" s="57">
+      <c r="N48" s="58">
         <f>N44-N47</f>
         <v>-6.2531375000000082</v>
       </c>
-      <c r="O48" s="57">
+      <c r="O48" s="58">
         <f>O44-O47</f>
         <v>-8.278490000000005</v>
       </c>
-      <c r="P48" s="59">
+      <c r="P48" s="60">
         <f>P44-P47</f>
         <v>-107.60099749999995</v>
       </c>
@@ -2733,8 +2740,8 @@
         <v>You would save $107.60 by using Flat Rate pricing</v>
       </c>
     </row>
-    <row r="49" spans="2:18" s="53" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C49" s="54"/>
+    <row r="49" spans="2:18" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="C49" s="55"/>
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
@@ -2922,10 +2929,10 @@
       </c>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D60" s="56"/>
+      <c r="D60" s="57"/>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D61" s="56"/>
+      <c r="D61" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>